<commit_message>
Add a new unit test to check for empty transition names in the Transition_Name_Annot sheet.
</commit_message>
<xml_diff>
--- a/tests/testdata/test_transition_annot/WideTableForm_Annotation.xlsx
+++ b/tests/testdata/test_transition_annot/WideTableForm_Annotation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MSOrganiser\tests\testdata\test_istd_annot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MSOrganiser\tests\testdata\test_transition_annot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E8660F-51E5-4E63-B20A-A7EB19207008}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F74A687-5982-456A-8B25-83E61EBFCFFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16770" windowHeight="8775" xr2:uid="{99D2A2AC-8431-4E91-B3F6-6736E2B6E0B0}"/>
   </bookViews>

</xml_diff>